<commit_message>
updated column structure file
</commit_message>
<xml_diff>
--- a/c_gigas_transcriptome_SRA_bioprojects_updated_column_structure.xlsx
+++ b/c_gigas_transcriptome_SRA_bioprojects_updated_column_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24140" windowHeight="21440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Full_Data" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="425">
   <si>
     <t>Larvae</t>
   </si>
@@ -589,15 +589,6 @@
   </si>
   <si>
     <t>SRR796592</t>
-  </si>
-  <si>
-    <t>PBS</t>
-  </si>
-  <si>
-    <t>710.1M</t>
-  </si>
-  <si>
-    <t>SRR796591</t>
   </si>
   <si>
     <t>734.4M</t>
@@ -1418,7 +1409,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="368">
+  <cellStyleXfs count="371">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1437,6 +1428,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1803,7 +1797,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="368">
+  <cellStyles count="371">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2162,6 +2156,9 @@
     <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2500,10 +2497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q156"/>
+  <dimension ref="A1:Q155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="H138" sqref="H137:H138"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="N135" sqref="N135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2518,7 +2515,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="21">
       <c r="A1" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2578,16 +2575,16 @@
     <row r="4" spans="1:17">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>12</v>
@@ -2611,10 +2608,10 @@
         <v>13</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -2625,13 +2622,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>26</v>
@@ -2658,10 +2655,10 @@
         <v>16</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -2672,16 +2669,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>354</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>357</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>2</v>
@@ -2708,7 +2705,7 @@
         <v>46</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -2719,13 +2716,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>26</v>
@@ -2752,10 +2749,10 @@
         <v>16</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -2766,16 +2763,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>2</v>
@@ -2802,7 +2799,7 @@
         <v>48</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -2813,13 +2810,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>26</v>
@@ -2846,10 +2843,10 @@
         <v>16</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -2860,16 +2857,16 @@
         <v>2</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>2</v>
@@ -2896,7 +2893,7 @@
         <v>50</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -2907,16 +2904,16 @@
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>3</v>
@@ -2943,7 +2940,7 @@
         <v>58</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -2954,13 +2951,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>26</v>
@@ -2987,10 +2984,10 @@
         <v>24</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -3001,16 +2998,16 @@
         <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>3</v>
@@ -3037,7 +3034,7 @@
         <v>62</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -3048,16 +3045,16 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>3</v>
@@ -3084,7 +3081,7 @@
         <v>66</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -3095,16 +3092,16 @@
         <v>4</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>3</v>
@@ -3131,7 +3128,7 @@
         <v>73</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -3142,16 +3139,16 @@
         <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>3</v>
@@ -3178,7 +3175,7 @@
         <v>62</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -3189,13 +3186,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>26</v>
@@ -3222,10 +3219,10 @@
         <v>24</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -3236,16 +3233,16 @@
         <v>4</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>3</v>
@@ -3272,7 +3269,7 @@
         <v>62</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -3283,16 +3280,16 @@
         <v>4</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>3</v>
@@ -3319,7 +3316,7 @@
         <v>53</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -3330,16 +3327,16 @@
         <v>4</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>3</v>
@@ -3366,7 +3363,7 @@
         <v>66</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -3377,13 +3374,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>26</v>
@@ -3410,10 +3407,10 @@
         <v>24</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -3424,16 +3421,16 @@
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>3</v>
@@ -3460,7 +3457,7 @@
         <v>73</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -3471,13 +3468,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>26</v>
@@ -3504,10 +3501,10 @@
         <v>24</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -3518,16 +3515,16 @@
         <v>4</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>3</v>
@@ -3554,7 +3551,7 @@
         <v>53</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -3565,13 +3562,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>26</v>
@@ -3598,10 +3595,10 @@
         <v>24</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -3612,16 +3609,16 @@
         <v>4</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>3</v>
@@ -3648,7 +3645,7 @@
         <v>64</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -3659,16 +3656,16 @@
         <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>3</v>
@@ -3695,7 +3692,7 @@
         <v>73</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -3706,16 +3703,16 @@
         <v>4</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>3</v>
@@ -3742,7 +3739,7 @@
         <v>66</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -3753,16 +3750,16 @@
         <v>4</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>3</v>
@@ -3789,7 +3786,7 @@
         <v>53</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -3800,16 +3797,16 @@
         <v>4</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>3</v>
@@ -3836,7 +3833,7 @@
         <v>58</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -3847,16 +3844,16 @@
         <v>4</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>3</v>
@@ -3883,7 +3880,7 @@
         <v>64</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -3894,13 +3891,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>26</v>
@@ -3927,10 +3924,10 @@
         <v>24</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
@@ -3941,16 +3938,16 @@
         <v>4</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>3</v>
@@ -3977,7 +3974,7 @@
         <v>58</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
@@ -3988,16 +3985,16 @@
         <v>4</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>3</v>
@@ -4024,7 +4021,7 @@
         <v>62</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -4038,10 +4035,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>80</v>
@@ -4085,10 +4082,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>83</v>
@@ -4132,10 +4129,10 @@
         <v>1</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>80</v>
@@ -4179,13 +4176,13 @@
         <v>1</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>4</v>
@@ -4209,10 +4206,10 @@
         <v>76</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -4226,13 +4223,13 @@
         <v>1</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>4</v>
@@ -4256,10 +4253,10 @@
         <v>76</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
@@ -4273,13 +4270,13 @@
         <v>1</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>4</v>
@@ -4303,10 +4300,10 @@
         <v>76</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -4320,10 +4317,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>96</v>
@@ -4367,10 +4364,10 @@
         <v>1</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>99</v>
@@ -4414,10 +4411,10 @@
         <v>1</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>103</v>
@@ -4461,10 +4458,10 @@
         <v>1</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>105</v>
@@ -4491,10 +4488,10 @@
         <v>76</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
@@ -4508,10 +4505,10 @@
         <v>1</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>108</v>
@@ -4538,10 +4535,10 @@
         <v>76</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
@@ -4555,10 +4552,10 @@
         <v>1</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>111</v>
@@ -4585,10 +4582,10 @@
         <v>76</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
@@ -4602,10 +4599,10 @@
         <v>1</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>114</v>
@@ -4649,10 +4646,10 @@
         <v>1</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>117</v>
@@ -4696,10 +4693,10 @@
         <v>1</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>120</v>
@@ -4743,10 +4740,10 @@
         <v>1</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>124</v>
@@ -4773,10 +4770,10 @@
         <v>76</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N50" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
@@ -4790,10 +4787,10 @@
         <v>1</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>127</v>
@@ -4820,10 +4817,10 @@
         <v>76</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
@@ -4837,10 +4834,10 @@
         <v>1</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>129</v>
@@ -4867,10 +4864,10 @@
         <v>76</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
@@ -4884,10 +4881,10 @@
         <v>1</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>132</v>
@@ -4931,10 +4928,10 @@
         <v>1</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>135</v>
@@ -4978,10 +4975,10 @@
         <v>1</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>137</v>
@@ -5025,10 +5022,10 @@
         <v>1</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>140</v>
@@ -5055,10 +5052,10 @@
         <v>76</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N56" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
@@ -5072,10 +5069,10 @@
         <v>1</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>142</v>
@@ -5102,10 +5099,10 @@
         <v>76</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
@@ -5119,10 +5116,10 @@
         <v>1</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>145</v>
@@ -5149,10 +5146,10 @@
         <v>76</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
@@ -5166,10 +5163,10 @@
         <v>1</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>148</v>
@@ -5213,10 +5210,10 @@
         <v>1</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>150</v>
@@ -5260,10 +5257,10 @@
         <v>1</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>153</v>
@@ -5307,13 +5304,13 @@
         <v>1</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>4</v>
@@ -5337,10 +5334,10 @@
         <v>76</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
@@ -5354,13 +5351,13 @@
         <v>1</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>4</v>
@@ -5384,10 +5381,10 @@
         <v>76</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
@@ -5401,13 +5398,13 @@
         <v>1</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D64" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E64" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>368</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>4</v>
@@ -5431,10 +5428,10 @@
         <v>76</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N64" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
@@ -5448,10 +5445,10 @@
         <v>0</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>26</v>
@@ -5478,10 +5475,10 @@
         <v>24</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
@@ -5495,13 +5492,13 @@
         <v>0</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>5</v>
@@ -5528,7 +5525,7 @@
         <v>165</v>
       </c>
       <c r="N66" s="7" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
@@ -5542,10 +5539,10 @@
         <v>1</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>168</v>
@@ -5575,7 +5572,7 @@
         <v>165</v>
       </c>
       <c r="N67" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
@@ -5589,10 +5586,10 @@
         <v>1</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>173</v>
@@ -5622,7 +5619,7 @@
         <v>165</v>
       </c>
       <c r="N68" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
@@ -5636,10 +5633,10 @@
         <v>1</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>175</v>
@@ -5669,7 +5666,7 @@
         <v>165</v>
       </c>
       <c r="N69" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
@@ -5683,10 +5680,10 @@
         <v>1</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>179</v>
@@ -5716,7 +5713,7 @@
         <v>165</v>
       </c>
       <c r="N70" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
@@ -5730,10 +5727,10 @@
         <v>1</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>181</v>
@@ -5763,7 +5760,7 @@
         <v>165</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
@@ -5777,10 +5774,10 @@
         <v>1</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>184</v>
@@ -5810,7 +5807,7 @@
         <v>165</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
@@ -5824,7 +5821,7 @@
         <v>1</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>187</v>
@@ -5857,7 +5854,7 @@
         <v>165</v>
       </c>
       <c r="N73" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
@@ -5871,13 +5868,13 @@
         <v>1</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>190</v>
+        <v>379</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>190</v>
+        <v>26</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>6</v>
@@ -5886,7 +5883,7 @@
         <v>9</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I74" s="4" t="s">
         <v>9</v>
@@ -5895,16 +5892,16 @@
         <v>169</v>
       </c>
       <c r="K74" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L74" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="M74" s="3" t="s">
-        <v>165</v>
+      <c r="M74" s="1" t="s">
+        <v>336</v>
       </c>
       <c r="N74" s="4" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
@@ -5912,46 +5909,46 @@
     </row>
     <row r="75" spans="1:17" ht="16">
       <c r="A75" s="4">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>383</v>
+        <v>347</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>26</v>
+        <v>385</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G75" s="5">
-        <v>9</v>
-      </c>
-      <c r="H75" s="9" t="s">
-        <v>194</v>
+        <v>112</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="I75" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="K75" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L75" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="M75" s="1" t="s">
-        <v>339</v>
+        <v>24</v>
+      </c>
+      <c r="M75" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="N75" s="4" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="O75" s="1"/>
       <c r="P75" s="1"/>
@@ -5965,13 +5962,13 @@
         <v>1</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>7</v>
@@ -5979,8 +5976,8 @@
       <c r="G76" s="5">
         <v>112</v>
       </c>
-      <c r="H76" s="4" t="s">
-        <v>196</v>
+      <c r="H76" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="I76" s="4" t="s">
         <v>9</v>
@@ -5989,16 +5986,16 @@
         <v>163</v>
       </c>
       <c r="K76" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L76" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N76" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
@@ -6012,13 +6009,13 @@
         <v>1</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>7</v>
@@ -6027,7 +6024,7 @@
         <v>112</v>
       </c>
       <c r="H77" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I77" s="4" t="s">
         <v>9</v>
@@ -6036,16 +6033,16 @@
         <v>163</v>
       </c>
       <c r="K77" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L77" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N77" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
@@ -6059,13 +6056,13 @@
         <v>1</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>7</v>
@@ -6074,7 +6071,7 @@
         <v>112</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I78" s="4" t="s">
         <v>9</v>
@@ -6083,16 +6080,16 @@
         <v>163</v>
       </c>
       <c r="K78" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L78" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M78" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="N78" s="4" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
@@ -6106,13 +6103,13 @@
         <v>1</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>7</v>
@@ -6121,7 +6118,7 @@
         <v>112</v>
       </c>
       <c r="H79" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I79" s="4" t="s">
         <v>9</v>
@@ -6130,16 +6127,16 @@
         <v>163</v>
       </c>
       <c r="K79" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L79" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M79" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N79" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O79" s="1"/>
       <c r="P79" s="1"/>
@@ -6153,13 +6150,13 @@
         <v>1</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>7</v>
@@ -6168,7 +6165,7 @@
         <v>112</v>
       </c>
       <c r="H80" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I80" s="4" t="s">
         <v>9</v>
@@ -6183,10 +6180,10 @@
         <v>24</v>
       </c>
       <c r="M80" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O80" s="1"/>
       <c r="P80" s="1"/>
@@ -6200,13 +6197,13 @@
         <v>1</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>7</v>
@@ -6224,16 +6221,16 @@
         <v>163</v>
       </c>
       <c r="K81" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L81" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N81" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
@@ -6247,13 +6244,13 @@
         <v>1</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>7</v>
@@ -6262,7 +6259,7 @@
         <v>112</v>
       </c>
       <c r="H82" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I82" s="4" t="s">
         <v>9</v>
@@ -6271,16 +6268,16 @@
         <v>163</v>
       </c>
       <c r="K82" s="5" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="L82" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M82" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N82" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O82" s="1"/>
       <c r="P82" s="1"/>
@@ -6294,13 +6291,13 @@
         <v>1</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>7</v>
@@ -6309,7 +6306,7 @@
         <v>112</v>
       </c>
       <c r="H83" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I83" s="4" t="s">
         <v>9</v>
@@ -6318,16 +6315,16 @@
         <v>163</v>
       </c>
       <c r="K83" s="5" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="L83" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M83" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N83" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O83" s="1"/>
       <c r="P83" s="1"/>
@@ -6341,13 +6338,13 @@
         <v>1</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>392</v>
+        <v>26</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>7</v>
@@ -6365,16 +6362,16 @@
         <v>163</v>
       </c>
       <c r="K84" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L84" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M84" s="3" t="s">
-        <v>213</v>
+      <c r="M84" s="1" t="s">
+        <v>336</v>
       </c>
       <c r="N84" s="4" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="O84" s="1"/>
       <c r="P84" s="1"/>
@@ -6388,10 +6385,10 @@
         <v>1</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>26</v>
@@ -6403,7 +6400,7 @@
         <v>112</v>
       </c>
       <c r="H85" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I85" s="4" t="s">
         <v>9</v>
@@ -6412,16 +6409,16 @@
         <v>163</v>
       </c>
       <c r="K85" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L85" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N85" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O85" s="1"/>
       <c r="P85" s="1"/>
@@ -6435,13 +6432,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>26</v>
+        <v>392</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>7</v>
@@ -6450,7 +6447,7 @@
         <v>112</v>
       </c>
       <c r="H86" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I86" s="4" t="s">
         <v>9</v>
@@ -6459,16 +6456,16 @@
         <v>163</v>
       </c>
       <c r="K86" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L86" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M86" s="1" t="s">
-        <v>339</v>
+      <c r="M86" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="N86" s="4" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="O86" s="1"/>
       <c r="P86" s="1"/>
@@ -6482,13 +6479,13 @@
         <v>1</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D87" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="E87" s="4" t="s">
         <v>394</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>395</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>7</v>
@@ -6497,7 +6494,7 @@
         <v>112</v>
       </c>
       <c r="H87" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I87" s="4" t="s">
         <v>9</v>
@@ -6506,16 +6503,16 @@
         <v>163</v>
       </c>
       <c r="K87" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L87" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M87" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N87" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O87" s="1"/>
       <c r="P87" s="1"/>
@@ -6529,13 +6526,13 @@
         <v>1</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="F88" s="5" t="s">
         <v>7</v>
@@ -6544,7 +6541,7 @@
         <v>112</v>
       </c>
       <c r="H88" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I88" s="4" t="s">
         <v>9</v>
@@ -6553,16 +6550,16 @@
         <v>163</v>
       </c>
       <c r="K88" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L88" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M88" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N88" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="O88" s="1"/>
       <c r="P88" s="1"/>
@@ -6576,13 +6573,13 @@
         <v>1</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="D89" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="E89" s="4" t="s">
         <v>394</v>
-      </c>
-      <c r="E89" s="4" t="s">
-        <v>395</v>
       </c>
       <c r="F89" s="5" t="s">
         <v>7</v>
@@ -6591,7 +6588,7 @@
         <v>112</v>
       </c>
       <c r="H89" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I89" s="4" t="s">
         <v>9</v>
@@ -6600,16 +6597,16 @@
         <v>163</v>
       </c>
       <c r="K89" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L89" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M89" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N89" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="O89" s="1"/>
       <c r="P89" s="1"/>
@@ -6623,13 +6620,13 @@
         <v>1</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F90" s="5" t="s">
         <v>7</v>
@@ -6638,7 +6635,7 @@
         <v>112</v>
       </c>
       <c r="H90" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I90" s="4" t="s">
         <v>9</v>
@@ -6647,16 +6644,16 @@
         <v>163</v>
       </c>
       <c r="K90" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L90" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M90" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="N90" s="4" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="O90" s="1"/>
       <c r="P90" s="1"/>
@@ -6670,13 +6667,13 @@
         <v>1</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="D91" s="12" t="s">
-        <v>398</v>
+        <v>348</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>396</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F91" s="5" t="s">
         <v>7</v>
@@ -6685,7 +6682,7 @@
         <v>112</v>
       </c>
       <c r="H91" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I91" s="4" t="s">
         <v>9</v>
@@ -6694,16 +6691,16 @@
         <v>163</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L91" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M91" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N91" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O91" s="1"/>
       <c r="P91" s="1"/>
@@ -6717,13 +6714,13 @@
         <v>1</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F92" s="5" t="s">
         <v>7</v>
@@ -6732,7 +6729,7 @@
         <v>112</v>
       </c>
       <c r="H92" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I92" s="4" t="s">
         <v>9</v>
@@ -6741,16 +6738,16 @@
         <v>163</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L92" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M92" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N92" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O92" s="1"/>
       <c r="P92" s="1"/>
@@ -6764,13 +6761,13 @@
         <v>1</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>7</v>
@@ -6779,7 +6776,7 @@
         <v>112</v>
       </c>
       <c r="H93" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I93" s="4" t="s">
         <v>9</v>
@@ -6788,16 +6785,16 @@
         <v>163</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L93" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M93" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N93" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="O93" s="1"/>
       <c r="P93" s="1"/>
@@ -6811,13 +6808,13 @@
         <v>1</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F94" s="5" t="s">
         <v>7</v>
@@ -6826,7 +6823,7 @@
         <v>112</v>
       </c>
       <c r="H94" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I94" s="4" t="s">
         <v>9</v>
@@ -6835,16 +6832,16 @@
         <v>163</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L94" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M94" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N94" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="O94" s="1"/>
       <c r="P94" s="1"/>
@@ -6858,13 +6855,13 @@
         <v>1</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F95" s="5" t="s">
         <v>7</v>
@@ -6873,7 +6870,7 @@
         <v>112</v>
       </c>
       <c r="H95" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I95" s="4" t="s">
         <v>9</v>
@@ -6882,16 +6879,16 @@
         <v>163</v>
       </c>
       <c r="K95" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L95" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M95" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N95" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="O95" s="1"/>
       <c r="P95" s="1"/>
@@ -6905,13 +6902,13 @@
         <v>1</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F96" s="5" t="s">
         <v>7</v>
@@ -6920,7 +6917,7 @@
         <v>112</v>
       </c>
       <c r="H96" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I96" s="4" t="s">
         <v>9</v>
@@ -6929,16 +6926,16 @@
         <v>163</v>
       </c>
       <c r="K96" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L96" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M96" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="N96" s="4" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="O96" s="1"/>
       <c r="P96" s="1"/>
@@ -6952,13 +6949,13 @@
         <v>1</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F97" s="5" t="s">
         <v>7</v>
@@ -6967,7 +6964,7 @@
         <v>112</v>
       </c>
       <c r="H97" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I97" s="4" t="s">
         <v>9</v>
@@ -6976,16 +6973,16 @@
         <v>163</v>
       </c>
       <c r="K97" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L97" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M97" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N97" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O97" s="1"/>
       <c r="P97" s="1"/>
@@ -6999,13 +6996,13 @@
         <v>1</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F98" s="5" t="s">
         <v>7</v>
@@ -7014,7 +7011,7 @@
         <v>112</v>
       </c>
       <c r="H98" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I98" s="4" t="s">
         <v>9</v>
@@ -7023,16 +7020,16 @@
         <v>163</v>
       </c>
       <c r="K98" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L98" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M98" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N98" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O98" s="1"/>
       <c r="P98" s="1"/>
@@ -7046,13 +7043,13 @@
         <v>1</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F99" s="5" t="s">
         <v>7</v>
@@ -7061,7 +7058,7 @@
         <v>112</v>
       </c>
       <c r="H99" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I99" s="4" t="s">
         <v>9</v>
@@ -7070,16 +7067,16 @@
         <v>163</v>
       </c>
       <c r="K99" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L99" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M99" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N99" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O99" s="1"/>
       <c r="P99" s="1"/>
@@ -7093,13 +7090,13 @@
         <v>1</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>399</v>
+        <v>243</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F100" s="5" t="s">
         <v>7</v>
@@ -7108,7 +7105,7 @@
         <v>112</v>
       </c>
       <c r="H100" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I100" s="4" t="s">
         <v>9</v>
@@ -7117,16 +7114,16 @@
         <v>163</v>
       </c>
       <c r="K100" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L100" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M100" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N100" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O100" s="1"/>
       <c r="P100" s="1"/>
@@ -7140,13 +7137,13 @@
         <v>1</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>246</v>
+        <v>391</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="F101" s="5" t="s">
         <v>7</v>
@@ -7170,10 +7167,10 @@
         <v>24</v>
       </c>
       <c r="M101" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N101" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="O101" s="1"/>
       <c r="P101" s="1"/>
@@ -7187,13 +7184,13 @@
         <v>1</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="D102" s="4" t="s">
-        <v>394</v>
+        <v>347</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>393</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F102" s="5" t="s">
         <v>7</v>
@@ -7202,7 +7199,7 @@
         <v>112</v>
       </c>
       <c r="H102" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I102" s="4" t="s">
         <v>9</v>
@@ -7211,16 +7208,16 @@
         <v>163</v>
       </c>
       <c r="K102" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L102" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M102" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N102" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="O102" s="1"/>
       <c r="P102" s="1"/>
@@ -7234,13 +7231,13 @@
         <v>1</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="D103" s="12" t="s">
-        <v>396</v>
+        <v>347</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>395</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F103" s="5" t="s">
         <v>7</v>
@@ -7249,7 +7246,7 @@
         <v>112</v>
       </c>
       <c r="H103" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I103" s="4" t="s">
         <v>9</v>
@@ -7258,16 +7255,16 @@
         <v>163</v>
       </c>
       <c r="K103" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L103" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M103" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N103" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="O103" s="1"/>
       <c r="P103" s="1"/>
@@ -7281,13 +7278,13 @@
         <v>1</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F104" s="5" t="s">
         <v>7</v>
@@ -7296,7 +7293,7 @@
         <v>112</v>
       </c>
       <c r="H104" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I104" s="4" t="s">
         <v>9</v>
@@ -7311,10 +7308,10 @@
         <v>24</v>
       </c>
       <c r="M104" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N104" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="O104" s="1"/>
       <c r="P104" s="1"/>
@@ -7328,13 +7325,13 @@
         <v>1</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F105" s="5" t="s">
         <v>7</v>
@@ -7352,16 +7349,16 @@
         <v>163</v>
       </c>
       <c r="K105" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="L105" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M105" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N105" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="O105" s="1"/>
       <c r="P105" s="1"/>
@@ -7375,13 +7372,13 @@
         <v>1</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="F106" s="5" t="s">
         <v>7</v>
@@ -7390,7 +7387,7 @@
         <v>112</v>
       </c>
       <c r="H106" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I106" s="4" t="s">
         <v>9</v>
@@ -7399,16 +7396,16 @@
         <v>163</v>
       </c>
       <c r="K106" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L106" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M106" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N106" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="O106" s="1"/>
       <c r="P106" s="1"/>
@@ -7422,13 +7419,13 @@
         <v>1</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="F107" s="5" t="s">
         <v>7</v>
@@ -7437,7 +7434,7 @@
         <v>112</v>
       </c>
       <c r="H107" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I107" s="4" t="s">
         <v>9</v>
@@ -7446,16 +7443,16 @@
         <v>163</v>
       </c>
       <c r="K107" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L107" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M107" s="3" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="N107" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="O107" s="1"/>
       <c r="P107" s="1"/>
@@ -7469,13 +7466,13 @@
         <v>1</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F108" s="5" t="s">
         <v>7</v>
@@ -7484,7 +7481,7 @@
         <v>112</v>
       </c>
       <c r="H108" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I108" s="4" t="s">
         <v>9</v>
@@ -7493,16 +7490,16 @@
         <v>163</v>
       </c>
       <c r="K108" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L108" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M108" s="3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="N108" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="O108" s="1"/>
       <c r="P108" s="1"/>
@@ -7516,13 +7513,13 @@
         <v>1</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>406</v>
+        <v>381</v>
       </c>
       <c r="F109" s="5" t="s">
         <v>7</v>
@@ -7531,7 +7528,7 @@
         <v>112</v>
       </c>
       <c r="H109" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I109" s="4" t="s">
         <v>9</v>
@@ -7540,16 +7537,16 @@
         <v>163</v>
       </c>
       <c r="K109" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L109" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M109" s="3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="N109" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="O109" s="1"/>
       <c r="P109" s="1"/>
@@ -7563,13 +7560,13 @@
         <v>1</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F110" s="5" t="s">
         <v>7</v>
@@ -7578,7 +7575,7 @@
         <v>112</v>
       </c>
       <c r="H110" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I110" s="4" t="s">
         <v>9</v>
@@ -7587,16 +7584,16 @@
         <v>163</v>
       </c>
       <c r="K110" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L110" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M110" s="3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="N110" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="O110" s="1"/>
       <c r="P110" s="1"/>
@@ -7610,13 +7607,13 @@
         <v>1</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F111" s="5" t="s">
         <v>7</v>
@@ -7625,7 +7622,7 @@
         <v>112</v>
       </c>
       <c r="H111" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I111" s="4" t="s">
         <v>9</v>
@@ -7640,10 +7637,10 @@
         <v>24</v>
       </c>
       <c r="M111" s="3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="N111" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="O111" s="1"/>
       <c r="P111" s="1"/>
@@ -7657,13 +7654,13 @@
         <v>1</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>386</v>
+        <v>404</v>
       </c>
       <c r="F112" s="5" t="s">
         <v>7</v>
@@ -7681,16 +7678,16 @@
         <v>163</v>
       </c>
       <c r="K112" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="L112" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M112" s="3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="N112" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="O112" s="1"/>
       <c r="P112" s="1"/>
@@ -7704,13 +7701,13 @@
         <v>1</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F113" s="5" t="s">
         <v>7</v>
@@ -7719,7 +7716,7 @@
         <v>112</v>
       </c>
       <c r="H113" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I113" s="4" t="s">
         <v>9</v>
@@ -7728,16 +7725,16 @@
         <v>163</v>
       </c>
       <c r="K113" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L113" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M113" s="3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="N113" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="O113" s="1"/>
       <c r="P113" s="1"/>
@@ -7751,13 +7748,13 @@
         <v>1</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F114" s="5" t="s">
         <v>7</v>
@@ -7766,7 +7763,7 @@
         <v>112</v>
       </c>
       <c r="H114" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I114" s="4" t="s">
         <v>9</v>
@@ -7781,10 +7778,10 @@
         <v>24</v>
       </c>
       <c r="M114" s="3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="N114" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="O114" s="1"/>
       <c r="P114" s="1"/>
@@ -7798,13 +7795,13 @@
         <v>1</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="F115" s="5" t="s">
         <v>7</v>
@@ -7822,16 +7819,16 @@
         <v>163</v>
       </c>
       <c r="K115" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L115" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M115" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="N115" s="4" t="s">
-        <v>333</v>
+        <v>316</v>
+      </c>
+      <c r="N115" s="7" t="s">
+        <v>331</v>
       </c>
       <c r="O115" s="1"/>
       <c r="P115" s="1"/>
@@ -7845,13 +7842,13 @@
         <v>1</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E116" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F116" s="5" t="s">
         <v>7</v>
@@ -7860,7 +7857,7 @@
         <v>112</v>
       </c>
       <c r="H116" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I116" s="4" t="s">
         <v>9</v>
@@ -7869,16 +7866,16 @@
         <v>163</v>
       </c>
       <c r="K116" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L116" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M116" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N116" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="O116" s="1"/>
       <c r="P116" s="1"/>
@@ -7892,13 +7889,13 @@
         <v>1</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>406</v>
+        <v>381</v>
       </c>
       <c r="F117" s="5" t="s">
         <v>7</v>
@@ -7907,7 +7904,7 @@
         <v>112</v>
       </c>
       <c r="H117" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I117" s="4" t="s">
         <v>9</v>
@@ -7916,16 +7913,16 @@
         <v>163</v>
       </c>
       <c r="K117" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L117" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M117" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N117" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="O117" s="1"/>
       <c r="P117" s="1"/>
@@ -7939,13 +7936,13 @@
         <v>1</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F118" s="5" t="s">
         <v>7</v>
@@ -7954,7 +7951,7 @@
         <v>112</v>
       </c>
       <c r="H118" s="9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I118" s="4" t="s">
         <v>9</v>
@@ -7969,10 +7966,10 @@
         <v>24</v>
       </c>
       <c r="M118" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N118" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="O118" s="1"/>
       <c r="P118" s="1"/>
@@ -7986,13 +7983,13 @@
         <v>1</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F119" s="5" t="s">
         <v>7</v>
@@ -8001,7 +7998,7 @@
         <v>112</v>
       </c>
       <c r="H119" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I119" s="4" t="s">
         <v>9</v>
@@ -8010,16 +8007,16 @@
         <v>163</v>
       </c>
       <c r="K119" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L119" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M119" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N119" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="O119" s="1"/>
       <c r="P119" s="1"/>
@@ -8033,13 +8030,13 @@
         <v>1</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>386</v>
+        <v>404</v>
       </c>
       <c r="F120" s="5" t="s">
         <v>7</v>
@@ -8048,7 +8045,7 @@
         <v>112</v>
       </c>
       <c r="H120" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I120" s="4" t="s">
         <v>9</v>
@@ -8057,20 +8054,17 @@
         <v>163</v>
       </c>
       <c r="K120" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L120" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M120" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N120" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="O120" s="1"/>
-      <c r="P120" s="1"/>
-      <c r="Q120" s="1"/>
+        <v>331</v>
+      </c>
     </row>
     <row r="121" spans="1:17" ht="16">
       <c r="A121" s="4">
@@ -8080,13 +8074,13 @@
         <v>1</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F121" s="5" t="s">
         <v>7</v>
@@ -8095,7 +8089,7 @@
         <v>112</v>
       </c>
       <c r="H121" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I121" s="4" t="s">
         <v>9</v>
@@ -8104,16 +8098,16 @@
         <v>163</v>
       </c>
       <c r="K121" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L121" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M121" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N121" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="122" spans="1:17" ht="16">
@@ -8124,10 +8118,10 @@
         <v>1</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E122" s="4" t="s">
         <v>408</v>
@@ -8139,7 +8133,7 @@
         <v>112</v>
       </c>
       <c r="H122" s="9" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="I122" s="4" t="s">
         <v>9</v>
@@ -8154,10 +8148,10 @@
         <v>24</v>
       </c>
       <c r="M122" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N122" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="123" spans="1:17" ht="16">
@@ -8168,13 +8162,13 @@
         <v>1</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F123" s="5" t="s">
         <v>7</v>
@@ -8183,7 +8177,7 @@
         <v>112</v>
       </c>
       <c r="H123" s="9" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="I123" s="4" t="s">
         <v>9</v>
@@ -8192,16 +8186,16 @@
         <v>163</v>
       </c>
       <c r="K123" s="5" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="L123" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M123" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N123" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="124" spans="1:17" ht="16">
@@ -8212,13 +8206,13 @@
         <v>1</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E124" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F124" s="5" t="s">
         <v>7</v>
@@ -8235,17 +8229,17 @@
       <c r="J124" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="K124" s="5" t="s">
-        <v>290</v>
+      <c r="K124" s="10" t="s">
+        <v>295</v>
       </c>
       <c r="L124" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M124" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N124" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="125" spans="1:17" ht="16">
@@ -8256,13 +8250,13 @@
         <v>1</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F125" s="5" t="s">
         <v>7</v>
@@ -8271,7 +8265,7 @@
         <v>112</v>
       </c>
       <c r="H125" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I125" s="4" t="s">
         <v>9</v>
@@ -8280,16 +8274,16 @@
         <v>163</v>
       </c>
       <c r="K125" s="10" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="L125" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M125" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N125" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="126" spans="1:17" ht="16">
@@ -8300,13 +8294,13 @@
         <v>1</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F126" s="5" t="s">
         <v>7</v>
@@ -8315,7 +8309,7 @@
         <v>112</v>
       </c>
       <c r="H126" s="9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I126" s="4" t="s">
         <v>9</v>
@@ -8323,17 +8317,17 @@
       <c r="J126" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="K126" s="10" t="s">
-        <v>297</v>
+      <c r="K126" s="5" t="s">
+        <v>293</v>
       </c>
       <c r="L126" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M126" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N126" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="127" spans="1:17" ht="16">
@@ -8344,13 +8338,13 @@
         <v>1</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F127" s="5" t="s">
         <v>7</v>
@@ -8359,7 +8353,7 @@
         <v>112</v>
       </c>
       <c r="H127" s="9" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="I127" s="4" t="s">
         <v>9</v>
@@ -8368,16 +8362,16 @@
         <v>163</v>
       </c>
       <c r="K127" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L127" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M127" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N127" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="128" spans="1:17" ht="16">
@@ -8388,13 +8382,13 @@
         <v>1</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F128" s="5" t="s">
         <v>7</v>
@@ -8403,7 +8397,7 @@
         <v>112</v>
       </c>
       <c r="H128" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I128" s="4" t="s">
         <v>9</v>
@@ -8412,16 +8406,16 @@
         <v>163</v>
       </c>
       <c r="K128" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L128" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M128" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N128" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="129" spans="1:17" ht="16">
@@ -8432,10 +8426,10 @@
         <v>1</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>417</v>
@@ -8447,7 +8441,7 @@
         <v>112</v>
       </c>
       <c r="H129" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I129" s="4" t="s">
         <v>9</v>
@@ -8456,16 +8450,16 @@
         <v>163</v>
       </c>
       <c r="K129" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L129" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M129" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N129" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="130" spans="1:17" ht="16">
@@ -8476,13 +8470,13 @@
         <v>1</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F130" s="5" t="s">
         <v>7</v>
@@ -8491,7 +8485,7 @@
         <v>112</v>
       </c>
       <c r="H130" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I130" s="4" t="s">
         <v>9</v>
@@ -8500,16 +8494,16 @@
         <v>163</v>
       </c>
       <c r="K130" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L130" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M130" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N130" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="131" spans="1:17" ht="16">
@@ -8520,13 +8514,13 @@
         <v>1</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F131" s="5" t="s">
         <v>7</v>
@@ -8535,7 +8529,7 @@
         <v>112</v>
       </c>
       <c r="H131" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I131" s="4" t="s">
         <v>9</v>
@@ -8544,16 +8538,16 @@
         <v>163</v>
       </c>
       <c r="K131" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L131" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M131" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N131" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="132" spans="1:17" ht="16">
@@ -8564,13 +8558,13 @@
         <v>1</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F132" s="5" t="s">
         <v>7</v>
@@ -8579,7 +8573,7 @@
         <v>112</v>
       </c>
       <c r="H132" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I132" s="4" t="s">
         <v>9</v>
@@ -8588,16 +8582,16 @@
         <v>163</v>
       </c>
       <c r="K132" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L132" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M132" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N132" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="133" spans="1:17" ht="16">
@@ -8608,13 +8602,13 @@
         <v>1</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F133" s="5" t="s">
         <v>7</v>
@@ -8623,7 +8617,7 @@
         <v>112</v>
       </c>
       <c r="H133" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I133" s="4" t="s">
         <v>9</v>
@@ -8632,16 +8626,13 @@
         <v>163</v>
       </c>
       <c r="K133" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L133" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M133" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="N133" s="7" t="s">
-        <v>334</v>
+      <c r="M133" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="134" spans="1:17" ht="16">
@@ -8652,13 +8643,13 @@
         <v>1</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F134" s="5" t="s">
         <v>7</v>
@@ -8676,13 +8667,16 @@
         <v>163</v>
       </c>
       <c r="K134" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="L134" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M134" t="s">
-        <v>340</v>
+      <c r="M134" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="N134" s="4" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="135" spans="1:17" ht="16">
@@ -8693,13 +8687,13 @@
         <v>1</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F135" s="5" t="s">
         <v>7</v>
@@ -8708,7 +8702,7 @@
         <v>112</v>
       </c>
       <c r="H135" s="9" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I135" s="4" t="s">
         <v>9</v>
@@ -8723,27 +8717,27 @@
         <v>24</v>
       </c>
       <c r="M135" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N135" s="4" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="136" spans="1:17" ht="16">
       <c r="A136" s="4">
         <v>20</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B136" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="E136" s="4" t="s">
-        <v>426</v>
+        <v>26</v>
       </c>
       <c r="F136" s="5" t="s">
         <v>7</v>
@@ -8752,39 +8746,42 @@
         <v>112</v>
       </c>
       <c r="H136" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="I136" s="4" t="s">
-        <v>9</v>
+        <v>316</v>
+      </c>
+      <c r="I136" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="J136" s="4" t="s">
         <v>163</v>
       </c>
       <c r="K136" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L136" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M136" s="3" t="s">
-        <v>319</v>
+      <c r="M136" s="1" t="s">
+        <v>336</v>
       </c>
       <c r="N136" s="4" t="s">
-        <v>334</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="O136" s="1"/>
+      <c r="P136" s="1"/>
+      <c r="Q136" s="1"/>
     </row>
     <row r="137" spans="1:17" ht="16">
       <c r="A137" s="4">
         <v>20</v>
       </c>
       <c r="B137" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C137" s="4" t="s">
-        <v>350</v>
+        <v>341</v>
+      </c>
+      <c r="C137" s="12" t="s">
+        <v>349</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>26</v>
@@ -8796,7 +8793,7 @@
         <v>112</v>
       </c>
       <c r="H137" s="9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I137" s="11" t="s">
         <v>10</v>
@@ -8805,67 +8802,34 @@
         <v>163</v>
       </c>
       <c r="K137" s="5" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="L137" s="5" t="s">
         <v>24</v>
       </c>
       <c r="M137" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N137" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="O137" s="1"/>
       <c r="P137" s="1"/>
       <c r="Q137" s="1"/>
     </row>
-    <row r="138" spans="1:17" ht="16">
-      <c r="A138" s="4">
-        <v>20</v>
-      </c>
-      <c r="B138" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="C138" s="12" t="s">
-        <v>352</v>
-      </c>
-      <c r="D138" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="E138" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F138" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G138" s="5">
-        <v>112</v>
-      </c>
-      <c r="H138" s="9" t="s">
-        <v>320</v>
-      </c>
-      <c r="I138" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J138" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="K138" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="L138" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M138" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="N138" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="O138" s="1"/>
-      <c r="P138" s="1"/>
-      <c r="Q138" s="1"/>
+    <row r="138" spans="1:17">
+      <c r="A138" s="8"/>
+      <c r="B138" s="8"/>
+      <c r="C138" s="8"/>
+      <c r="D138" s="8"/>
+      <c r="E138" s="8"/>
+      <c r="F138" s="8"/>
+      <c r="G138" s="8"/>
+      <c r="H138" s="8"/>
+      <c r="I138" s="8"/>
+      <c r="J138" s="8"/>
+      <c r="K138" s="8"/>
+      <c r="L138" s="8"/>
     </row>
     <row r="139" spans="1:17">
       <c r="A139" s="8"/>
@@ -9104,20 +9068,6 @@
       <c r="J155" s="8"/>
       <c r="K155" s="8"/>
       <c r="L155" s="8"/>
-    </row>
-    <row r="156" spans="1:12">
-      <c r="A156" s="8"/>
-      <c r="B156" s="8"/>
-      <c r="C156" s="8"/>
-      <c r="D156" s="8"/>
-      <c r="E156" s="8"/>
-      <c r="F156" s="8"/>
-      <c r="G156" s="8"/>
-      <c r="H156" s="8"/>
-      <c r="I156" s="8"/>
-      <c r="J156" s="8"/>
-      <c r="K156" s="8"/>
-      <c r="L156" s="8"/>
     </row>
   </sheetData>
   <sortState ref="L1:L1048576">
@@ -9189,7 +9139,7 @@
     <hyperlink ref="H72" r:id="rId63"/>
     <hyperlink ref="H73" r:id="rId64"/>
     <hyperlink ref="H74" r:id="rId65"/>
-    <hyperlink ref="H75" r:id="rId66"/>
+    <hyperlink ref="H76" r:id="rId66"/>
     <hyperlink ref="H77" r:id="rId67"/>
     <hyperlink ref="H78" r:id="rId68"/>
     <hyperlink ref="H79" r:id="rId69"/>
@@ -9235,10 +9185,10 @@
     <hyperlink ref="H119" r:id="rId109"/>
     <hyperlink ref="H120" r:id="rId110"/>
     <hyperlink ref="H121" r:id="rId111"/>
-    <hyperlink ref="H122" r:id="rId112"/>
+    <hyperlink ref="H123" r:id="rId112"/>
     <hyperlink ref="H124" r:id="rId113"/>
-    <hyperlink ref="H125" r:id="rId114"/>
-    <hyperlink ref="H123" r:id="rId115"/>
+    <hyperlink ref="H122" r:id="rId114"/>
+    <hyperlink ref="H125" r:id="rId115"/>
     <hyperlink ref="H126" r:id="rId116"/>
     <hyperlink ref="H127" r:id="rId117"/>
     <hyperlink ref="H128" r:id="rId118"/>
@@ -9249,53 +9199,53 @@
     <hyperlink ref="H133" r:id="rId123"/>
     <hyperlink ref="H134" r:id="rId124"/>
     <hyperlink ref="H135" r:id="rId125"/>
-    <hyperlink ref="H136" r:id="rId126"/>
-    <hyperlink ref="M6" r:id="rId127"/>
-    <hyperlink ref="M8" r:id="rId128"/>
-    <hyperlink ref="M11" r:id="rId129"/>
-    <hyperlink ref="M13" r:id="rId130"/>
-    <hyperlink ref="M14" r:id="rId131"/>
-    <hyperlink ref="M15" r:id="rId132"/>
-    <hyperlink ref="M16" r:id="rId133"/>
-    <hyperlink ref="M10" r:id="rId134"/>
-    <hyperlink ref="M18" r:id="rId135"/>
-    <hyperlink ref="M19" r:id="rId136"/>
-    <hyperlink ref="M20" r:id="rId137"/>
-    <hyperlink ref="M22" r:id="rId138"/>
-    <hyperlink ref="M24" r:id="rId139"/>
-    <hyperlink ref="M26" r:id="rId140"/>
-    <hyperlink ref="M27" r:id="rId141"/>
-    <hyperlink ref="M28" r:id="rId142"/>
-    <hyperlink ref="M29" r:id="rId143"/>
-    <hyperlink ref="M30" r:id="rId144"/>
-    <hyperlink ref="M31" r:id="rId145"/>
-    <hyperlink ref="M33" r:id="rId146"/>
-    <hyperlink ref="M34" r:id="rId147"/>
-    <hyperlink ref="M66" r:id="rId148"/>
-    <hyperlink ref="M37" r:id="rId149"/>
-    <hyperlink ref="M35" r:id="rId150"/>
-    <hyperlink ref="M43" r:id="rId151"/>
-    <hyperlink ref="M41" r:id="rId152"/>
-    <hyperlink ref="M42" r:id="rId153"/>
-    <hyperlink ref="M48" r:id="rId154"/>
-    <hyperlink ref="M53" r:id="rId155"/>
-    <hyperlink ref="M54" r:id="rId156"/>
-    <hyperlink ref="M55" r:id="rId157"/>
-    <hyperlink ref="M61" r:id="rId158"/>
-    <hyperlink ref="M60" r:id="rId159"/>
-    <hyperlink ref="M59" r:id="rId160"/>
-    <hyperlink ref="M67:M74" r:id="rId161" display="SRR960964"/>
+    <hyperlink ref="M6" r:id="rId126"/>
+    <hyperlink ref="M8" r:id="rId127"/>
+    <hyperlink ref="M11" r:id="rId128"/>
+    <hyperlink ref="M13" r:id="rId129"/>
+    <hyperlink ref="M14" r:id="rId130"/>
+    <hyperlink ref="M15" r:id="rId131"/>
+    <hyperlink ref="M16" r:id="rId132"/>
+    <hyperlink ref="M10" r:id="rId133"/>
+    <hyperlink ref="M18" r:id="rId134"/>
+    <hyperlink ref="M19" r:id="rId135"/>
+    <hyperlink ref="M20" r:id="rId136"/>
+    <hyperlink ref="M22" r:id="rId137"/>
+    <hyperlink ref="M24" r:id="rId138"/>
+    <hyperlink ref="M26" r:id="rId139"/>
+    <hyperlink ref="M27" r:id="rId140"/>
+    <hyperlink ref="M28" r:id="rId141"/>
+    <hyperlink ref="M29" r:id="rId142"/>
+    <hyperlink ref="M30" r:id="rId143"/>
+    <hyperlink ref="M31" r:id="rId144"/>
+    <hyperlink ref="M33" r:id="rId145"/>
+    <hyperlink ref="M34" r:id="rId146"/>
+    <hyperlink ref="M66" r:id="rId147"/>
+    <hyperlink ref="M37" r:id="rId148"/>
+    <hyperlink ref="M35" r:id="rId149"/>
+    <hyperlink ref="M43" r:id="rId150"/>
+    <hyperlink ref="M41" r:id="rId151"/>
+    <hyperlink ref="M42" r:id="rId152"/>
+    <hyperlink ref="M48" r:id="rId153"/>
+    <hyperlink ref="M53" r:id="rId154"/>
+    <hyperlink ref="M54" r:id="rId155"/>
+    <hyperlink ref="M55" r:id="rId156"/>
+    <hyperlink ref="M61" r:id="rId157"/>
+    <hyperlink ref="M60" r:id="rId158"/>
+    <hyperlink ref="M59" r:id="rId159"/>
+    <hyperlink ref="M67:M73" r:id="rId160" display="SRR960964"/>
+    <hyperlink ref="M75" r:id="rId161"/>
     <hyperlink ref="M76" r:id="rId162"/>
     <hyperlink ref="M77" r:id="rId163"/>
-    <hyperlink ref="M78" r:id="rId164"/>
+    <hyperlink ref="M79" r:id="rId164"/>
     <hyperlink ref="M80" r:id="rId165"/>
     <hyperlink ref="M81" r:id="rId166"/>
     <hyperlink ref="M82" r:id="rId167"/>
     <hyperlink ref="M83" r:id="rId168"/>
-    <hyperlink ref="M84" r:id="rId169"/>
+    <hyperlink ref="M86" r:id="rId169"/>
     <hyperlink ref="M87" r:id="rId170"/>
-    <hyperlink ref="M88" r:id="rId171"/>
-    <hyperlink ref="M79" r:id="rId172"/>
+    <hyperlink ref="M78" r:id="rId171"/>
+    <hyperlink ref="M88" r:id="rId172"/>
     <hyperlink ref="M89" r:id="rId173"/>
     <hyperlink ref="M90" r:id="rId174"/>
     <hyperlink ref="M91" r:id="rId175"/>
@@ -9314,29 +9264,29 @@
     <hyperlink ref="M104" r:id="rId188"/>
     <hyperlink ref="M105" r:id="rId189"/>
     <hyperlink ref="M106" r:id="rId190"/>
-    <hyperlink ref="M107" r:id="rId191"/>
-    <hyperlink ref="H137" r:id="rId192"/>
-    <hyperlink ref="M136" r:id="rId193"/>
-    <hyperlink ref="H138" r:id="rId194"/>
-    <hyperlink ref="M135" r:id="rId195"/>
-    <hyperlink ref="M133" r:id="rId196"/>
-    <hyperlink ref="M132" r:id="rId197"/>
-    <hyperlink ref="M131" r:id="rId198"/>
-    <hyperlink ref="M130" r:id="rId199"/>
-    <hyperlink ref="M129" r:id="rId200"/>
-    <hyperlink ref="M128" r:id="rId201"/>
-    <hyperlink ref="M127" r:id="rId202"/>
-    <hyperlink ref="M126" r:id="rId203"/>
-    <hyperlink ref="M125" r:id="rId204"/>
-    <hyperlink ref="M124" r:id="rId205"/>
-    <hyperlink ref="M123" r:id="rId206"/>
-    <hyperlink ref="M122" r:id="rId207"/>
-    <hyperlink ref="M121" r:id="rId208"/>
-    <hyperlink ref="M120" r:id="rId209"/>
-    <hyperlink ref="M119" r:id="rId210"/>
-    <hyperlink ref="M118" r:id="rId211"/>
-    <hyperlink ref="M117" r:id="rId212"/>
-    <hyperlink ref="M116" r:id="rId213"/>
+    <hyperlink ref="H136" r:id="rId191"/>
+    <hyperlink ref="M135" r:id="rId192"/>
+    <hyperlink ref="H137" r:id="rId193"/>
+    <hyperlink ref="M134" r:id="rId194"/>
+    <hyperlink ref="M132" r:id="rId195"/>
+    <hyperlink ref="M131" r:id="rId196"/>
+    <hyperlink ref="M130" r:id="rId197"/>
+    <hyperlink ref="M129" r:id="rId198"/>
+    <hyperlink ref="M128" r:id="rId199"/>
+    <hyperlink ref="M127" r:id="rId200"/>
+    <hyperlink ref="M126" r:id="rId201"/>
+    <hyperlink ref="M125" r:id="rId202"/>
+    <hyperlink ref="M124" r:id="rId203"/>
+    <hyperlink ref="M123" r:id="rId204"/>
+    <hyperlink ref="M122" r:id="rId205"/>
+    <hyperlink ref="M121" r:id="rId206"/>
+    <hyperlink ref="M120" r:id="rId207"/>
+    <hyperlink ref="M119" r:id="rId208"/>
+    <hyperlink ref="M118" r:id="rId209"/>
+    <hyperlink ref="M117" r:id="rId210"/>
+    <hyperlink ref="M116" r:id="rId211"/>
+    <hyperlink ref="M115" r:id="rId212"/>
+    <hyperlink ref="M107" r:id="rId213"/>
     <hyperlink ref="M108" r:id="rId214"/>
     <hyperlink ref="M109" r:id="rId215"/>
     <hyperlink ref="M110" r:id="rId216"/>
@@ -9344,7 +9294,6 @@
     <hyperlink ref="M112" r:id="rId218"/>
     <hyperlink ref="M113" r:id="rId219"/>
     <hyperlink ref="M114" r:id="rId220"/>
-    <hyperlink ref="M115" r:id="rId221"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
added python script to convert StringTie output into DESeq2 count matrices, updated scripts
</commit_message>
<xml_diff>
--- a/c_gigas_transcriptome_SRA_bioprojects_updated_column_structure.xlsx
+++ b/c_gigas_transcriptome_SRA_bioprojects_updated_column_structure.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24140" windowHeight="21440" tabRatio="500"/>
+    <workbookView xWindow="1260" yWindow="8160" windowWidth="25600" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Full_Data" sheetId="4" r:id="rId1"/>
+    <sheet name="osHV1_PHENO_DATA" sheetId="5" r:id="rId2"/>
+    <sheet name="bac_PHENO_DATA" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="425">
   <si>
     <t>Larvae</t>
   </si>
@@ -2499,8 +2501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="N135" sqref="N135"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9303,4 +9305,1790 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="16">
+      <c r="A1" s="4">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5">
+        <v>33</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16">
+      <c r="A2" s="4">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5">
+        <v>33</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="16">
+      <c r="A3" s="4">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5">
+        <v>33</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="16">
+      <c r="A4" s="4">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5">
+        <v>33</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="16">
+      <c r="A5" s="4">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>33</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="16">
+      <c r="A6" s="4">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5">
+        <v>33</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="16">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5">
+        <v>33</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="5">
+        <v>33</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="16">
+      <c r="A9" s="4">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="5">
+        <v>33</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="16">
+      <c r="A10" s="4">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="5">
+        <v>33</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="16">
+      <c r="A11" s="4">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="5">
+        <v>33</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="16">
+      <c r="A12" s="4">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="5">
+        <v>33</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="16">
+      <c r="A13" s="4">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5">
+        <v>33</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="16">
+      <c r="A14" s="4">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="5">
+        <v>33</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="16">
+      <c r="A15" s="4">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="5">
+        <v>33</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="16">
+      <c r="A16" s="4">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="5">
+        <v>33</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="16">
+      <c r="A17" s="4">
+        <v>6</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="5">
+        <v>33</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="16">
+      <c r="A18" s="4">
+        <v>6</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="5">
+        <v>33</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="16">
+      <c r="A19" s="4">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="5">
+        <v>33</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="16">
+      <c r="A20" s="4">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="5">
+        <v>33</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="16">
+      <c r="A21" s="4">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="5">
+        <v>33</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="16">
+      <c r="A22" s="4">
+        <v>6</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="5">
+        <v>33</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="16">
+      <c r="A23" s="4">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="5">
+        <v>33</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="16">
+      <c r="A24" s="4">
+        <v>6</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="5">
+        <v>33</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="16">
+      <c r="A25" s="4">
+        <v>6</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="5">
+        <v>33</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="16">
+      <c r="A26" s="4">
+        <v>6</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="5">
+        <v>33</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="16">
+      <c r="A27" s="4">
+        <v>6</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="5">
+        <v>33</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="16">
+      <c r="A28" s="4">
+        <v>6</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="5">
+        <v>33</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="16">
+      <c r="A29" s="4">
+        <v>6</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="5">
+        <v>33</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="16">
+      <c r="A30" s="4">
+        <v>6</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="5">
+        <v>33</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H1" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="H4" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H7" r:id="rId6"/>
+    <hyperlink ref="H8" r:id="rId7"/>
+    <hyperlink ref="H9" r:id="rId8"/>
+    <hyperlink ref="H10" r:id="rId9"/>
+    <hyperlink ref="H11" r:id="rId10"/>
+    <hyperlink ref="H12" r:id="rId11"/>
+    <hyperlink ref="H13" r:id="rId12"/>
+    <hyperlink ref="H17" r:id="rId13"/>
+    <hyperlink ref="H19" r:id="rId14"/>
+    <hyperlink ref="H20" r:id="rId15"/>
+    <hyperlink ref="H21" r:id="rId16"/>
+    <hyperlink ref="H22" r:id="rId17"/>
+    <hyperlink ref="H23" r:id="rId18"/>
+    <hyperlink ref="H24" r:id="rId19"/>
+    <hyperlink ref="H25" r:id="rId20"/>
+    <hyperlink ref="H26" r:id="rId21"/>
+    <hyperlink ref="H27" r:id="rId22"/>
+    <hyperlink ref="H28" r:id="rId23"/>
+    <hyperlink ref="H29" r:id="rId24"/>
+    <hyperlink ref="H30" r:id="rId25"/>
+    <hyperlink ref="M3" r:id="rId26"/>
+    <hyperlink ref="M1" r:id="rId27"/>
+    <hyperlink ref="M9" r:id="rId28"/>
+    <hyperlink ref="M7" r:id="rId29"/>
+    <hyperlink ref="M8" r:id="rId30"/>
+    <hyperlink ref="M14" r:id="rId31"/>
+    <hyperlink ref="M19" r:id="rId32"/>
+    <hyperlink ref="M20" r:id="rId33"/>
+    <hyperlink ref="M21" r:id="rId34"/>
+    <hyperlink ref="M27" r:id="rId35"/>
+    <hyperlink ref="M26" r:id="rId36"/>
+    <hyperlink ref="M25" r:id="rId37"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:17" ht="16">
+      <c r="A1" s="4">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5">
+        <v>9</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" ht="16">
+      <c r="A2" s="4">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5">
+        <v>9</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" ht="16">
+      <c r="A3" s="4">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="5">
+        <v>9</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" ht="16">
+      <c r="A4" s="4">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="5">
+        <v>9</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" ht="16">
+      <c r="A5" s="4">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="5">
+        <v>9</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" ht="16">
+      <c r="A6" s="4">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="5">
+        <v>9</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" ht="16">
+      <c r="A7" s="4">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5">
+        <v>9</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" ht="16">
+      <c r="A8" s="4">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="5">
+        <v>9</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H1" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="H4" r:id="rId4"/>
+    <hyperlink ref="H5" r:id="rId5"/>
+    <hyperlink ref="H6" r:id="rId6"/>
+    <hyperlink ref="H7" r:id="rId7"/>
+    <hyperlink ref="H8" r:id="rId8"/>
+    <hyperlink ref="M1:M7" r:id="rId9" display="SRR960964"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>